<commit_message>
Add: dev front + specs un peu
</commit_message>
<xml_diff>
--- a/specs/dico.xlsx
+++ b/specs/dico.xlsx
@@ -166,6 +166,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -187,6 +188,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -194,6 +196,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -238,16 +241,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,258 +383,258 @@
   </sheetPr>
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.02"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>